<commit_message>
modified test cases excel
Signed-off-by: Jemin <jemin272@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
+++ b/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Module</t>
   </si>
@@ -121,6 +121,24 @@
   </si>
   <si>
     <t>tick or untick popup comes up {applicant_id:, cancel_flag:'0'</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>checking the priority functionality</t>
+  </si>
+  <si>
+    <t>1. click on priorities option in the 1st date slot tab</t>
+  </si>
+  <si>
+    <t>unwanted pop up</t>
+  </si>
+  <si>
+    <t>priorities tab should work</t>
+  </si>
+  <si>
+    <t>pop up comes up showing the server is not working</t>
   </si>
 </sst>
 </file>
@@ -532,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -547,7 +565,7 @@
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="15">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -697,6 +715,29 @@
       </c>
       <c r="G7" s="11" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test cases excel sheet
Signed-off-by: Jemin <jemin272@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
+++ b/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
   <si>
     <t>Module</t>
   </si>
@@ -253,6 +253,24 @@
   </si>
   <si>
     <t>taking up the data of past applicant and printing notice based on that</t>
+  </si>
+  <si>
+    <t>refund</t>
+  </si>
+  <si>
+    <t>checking refund amount</t>
+  </si>
+  <si>
+    <t>1.cancel any applicant who has paid more than 1000</t>
+  </si>
+  <si>
+    <t>calculate amt of refund based on dates</t>
+  </si>
+  <si>
+    <t>1000*% based on time + extra amount paid as it is</t>
+  </si>
+  <si>
+    <t>total amt * %</t>
   </si>
 </sst>
 </file>
@@ -291,7 +309,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +320,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -345,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -370,6 +394,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,17 +689,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="73.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
   </cols>
@@ -824,7 +849,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -850,7 +875,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -928,7 +953,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -955,7 +980,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>19</v>
@@ -981,7 +1006,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>58</v>
@@ -1006,7 +1031,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -1033,7 +1058,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>29</v>
@@ -1058,7 +1083,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="12" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1085,7 +1110,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>14</v>
@@ -1104,6 +1129,32 @@
       </c>
       <c r="H17" s="11" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ppt, applicant.csv, test cases excel
Signed-off-by: Jemin <jemin272@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
+++ b/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
   <si>
     <t>Module</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>pop up comes up showing the server is not working</t>
-  </si>
-  <si>
-    <t>open</t>
   </si>
   <si>
     <t>closed</t>
@@ -277,7 +274,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -308,8 +305,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,12 +323,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -369,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -394,7 +391,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,7 +690,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -772,7 +770,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>14</v>
@@ -798,7 +796,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>19</v>
@@ -824,7 +822,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>14</v>
@@ -875,7 +873,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -901,8 +899,8 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>42</v>
+      <c r="B9" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>35</v>
@@ -911,24 +909,24 @@
         <v>36</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>42</v>
+      <c r="B10" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>35</v>
@@ -937,23 +935,23 @@
         <v>36</v>
       </c>
       <c r="E10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="G10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -963,68 +961,68 @@
         <v>36</v>
       </c>
       <c r="E11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="H11" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>42</v>
+      <c r="B12" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>42</v>
+      <c r="B13" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1">
@@ -1041,76 +1039,76 @@
         <v>36</v>
       </c>
       <c r="E14" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="H14" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>42</v>
+      <c r="B15" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="10" t="s">
+      <c r="H15" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="H16" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>42</v>
+      <c r="B17" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>14</v>
@@ -1122,13 +1120,13 @@
         <v>16</v>
       </c>
       <c r="F17" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="H17" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1">
@@ -1139,22 +1137,22 @@
         <v>41</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="H18" s="11" t="s">
         <v>83</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added bugs by jemin
Signed-off-by: Karthik <karthikbm01@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
+++ b/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthik\Documents\SD\software_new\software_development_cgu\Gila_Breath_Camp\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="150" yWindow="585" windowWidth="12135" windowHeight="4050"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="105">
   <si>
     <t>Module</t>
   </si>
@@ -268,13 +273,76 @@
   </si>
   <si>
     <t>total amt * %</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>dialogue box</t>
+  </si>
+  <si>
+    <t>prevent additional dialogue box pop up</t>
+  </si>
+  <si>
+    <t>1. check on the checkbox of prevent page from creating additional dialogue box in popup</t>
+  </si>
+  <si>
+    <t>pop of completion of that task should come up</t>
+  </si>
+  <si>
+    <t>after selecting prevent…, pop up doesn't show up</t>
+  </si>
+  <si>
+    <t>bunkhouses</t>
+  </si>
+  <si>
+    <t>assignment of bunkhouses</t>
+  </si>
+  <si>
+    <t>assignment of binkhouses</t>
+  </si>
+  <si>
+    <t>assignment should be done only after check-in is complete</t>
+  </si>
+  <si>
+    <t>assignment is done directly after registration is complete and applicant is admitted</t>
+  </si>
+  <si>
+    <t>refresh page</t>
+  </si>
+  <si>
+    <t>stay on same page after refresh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. complete any function and click submit, </t>
+  </si>
+  <si>
+    <t>submit click</t>
+  </si>
+  <si>
+    <t>remain in same page</t>
+  </si>
+  <si>
+    <t>moves to regestraion page always</t>
+  </si>
+  <si>
+    <t>cancel test meaningful</t>
+  </si>
+  <si>
+    <t>1. click on cancel page and see cancel field</t>
+  </si>
+  <si>
+    <t>cancel tab</t>
+  </si>
+  <si>
+    <t>meaningful sentence in cancel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -366,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -393,12 +461,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -445,7 +522,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -477,9 +554,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -511,6 +589,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -686,23 +765,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="76" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="71.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -728,7 +807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -748,7 +827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -765,7 +844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -791,7 +870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -817,7 +896,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -843,7 +922,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -869,7 +948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -895,7 +974,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -921,7 +1000,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -947,7 +1026,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -973,7 +1052,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -999,7 +1078,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1025,7 +1104,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1051,7 +1130,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1077,7 +1156,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1103,7 +1182,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1129,7 +1208,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1153,6 +1232,104 @@
       </c>
       <c r="H18" s="11" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated bugs list, ppt and applicant.csv
Signed-off-by: Jemin <jemin272@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
+++ b/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karthik\Documents\SD\software_new\software_development_cgu\Gila_Breath_Camp\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="150" yWindow="585" windowWidth="12135" windowHeight="4050"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t>Module</t>
   </si>
@@ -284,9 +279,6 @@
     <t>prevent additional dialogue box pop up</t>
   </si>
   <si>
-    <t>1. check on the checkbox of prevent page from creating additional dialogue box in popup</t>
-  </si>
-  <si>
     <t>pop of completion of that task should come up</t>
   </si>
   <si>
@@ -299,9 +291,6 @@
     <t>assignment of bunkhouses</t>
   </si>
   <si>
-    <t>assignment of binkhouses</t>
-  </si>
-  <si>
     <t>assignment should be done only after check-in is complete</t>
   </si>
   <si>
@@ -336,13 +325,34 @@
   </si>
   <si>
     <t>meaningful sentence in cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. check on the checkbox of prevent page from creating additional dialoguebox in popup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dialogue box popup </t>
+  </si>
+  <si>
+    <t>details not refreshing</t>
+  </si>
+  <si>
+    <t>1. check-in any of the accepted applicant, go to bunkhouse</t>
+  </si>
+  <si>
+    <t>updated record</t>
+  </si>
+  <si>
+    <t>if checked-In record should automatically show in bunkhouse</t>
+  </si>
+  <si>
+    <t>doesn't update the record till the time page is manually refreshed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -380,7 +390,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,7 +399,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -404,64 +426,62 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,7 +542,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -554,10 +574,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -589,7 +608,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -765,33 +783,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="76" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="63" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="7" max="7" width="59.7109375" customWidth="1"/>
     <col min="8" max="8" width="71.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -806,533 +827,595 @@
       <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="I1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="B3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="8">
         <v>123</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A9" s="12">
         <v>8</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A11" s="12">
         <v>10</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A12" s="12">
         <v>11</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A14" s="12">
         <v>13</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A16" s="12">
         <v>15</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="9" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A18" s="12">
         <v>17</v>
       </c>
-      <c r="B18" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="B18" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A19" s="12">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A20" s="12">
+        <v>19</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="12" t="s">
+      <c r="D20" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A21" s="12">
+        <v>20</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D20" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="C21" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="D21" s="12" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="12" t="s">
+      <c r="E21" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A22" s="12">
+        <v>21</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C21" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" t="s">
-        <v>97</v>
-      </c>
-      <c r="F21" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="C22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="E22" s="12" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="12" t="s">
+      <c r="F22" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A23" s="14">
+        <v>22</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" t="s">
-        <v>103</v>
-      </c>
-      <c r="G22" t="s">
-        <v>104</v>
+      <c r="C23" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added bugs and updated make_setup python
Signed-off-by: Jemin <jemin272@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
+++ b/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="127">
   <si>
     <t>Module</t>
   </si>
@@ -346,6 +346,57 @@
   </si>
   <si>
     <t>doesn't update the record till the time page is manually refreshed</t>
+  </si>
+  <si>
+    <t>make setup</t>
+  </si>
+  <si>
+    <t>testing the make setup</t>
+  </si>
+  <si>
+    <t>try running the make setup bat file</t>
+  </si>
+  <si>
+    <t>add absolute path</t>
+  </si>
+  <si>
+    <t>path should be dynamic</t>
+  </si>
+  <si>
+    <t>hard coded path for rohan's system</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>checking the update after certain level</t>
+  </si>
+  <si>
+    <t>check-in an applicant, and then go an update an information</t>
+  </si>
+  <si>
+    <t>check update function</t>
+  </si>
+  <si>
+    <t>all updates should not be allowed after a certain point</t>
+  </si>
+  <si>
+    <t>any info can updated at any point.</t>
+  </si>
+  <si>
+    <t>checking the update functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. go to any other date and type any applicant Id in update registration </t>
+  </si>
+  <si>
+    <t>update record in different date</t>
+  </si>
+  <si>
+    <t>applicant info for 1 time slot should not be shown in other slots</t>
+  </si>
+  <si>
+    <t>applicant information for time slot 2 showing in time slot 1 &amp; 3</t>
   </si>
 </sst>
 </file>
@@ -784,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1314,7 +1365,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>89</v>
@@ -1368,7 +1419,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>29</v>
@@ -1412,6 +1463,84 @@
       </c>
       <c r="H23" s="16" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A24" s="14">
+        <v>23</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A25" s="14">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1">
+      <c r="A26" s="14">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed first version of ppt
Signed-off-by: Rohan <rohan9969@gmail.com>
</commit_message>
<xml_diff>
--- a/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
+++ b/Gila_Breath_Camp/Documents/gila-breath-test-cases.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rohan\CGU\Fall 2016\Software Development\BitBucket\software_development_cgu\Gila_Breath_Camp\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="150" yWindow="585" windowWidth="12135" windowHeight="4050"/>
   </bookViews>
@@ -402,8 +407,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -467,7 +472,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -490,22 +495,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -530,9 +524,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,7 +585,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -625,9 +617,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -659,6 +669,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -834,14 +862,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
@@ -853,7 +881,7 @@
     <col min="8" max="8" width="71.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -880,7 +908,7 @@
       </c>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -905,7 +933,7 @@
       <c r="H2" s="12"/>
       <c r="I2" s="12"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -928,7 +956,7 @@
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -955,7 +983,7 @@
       </c>
       <c r="I4" s="12"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -982,7 +1010,7 @@
       </c>
       <c r="I5" s="12"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1009,7 +1037,7 @@
       </c>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1036,7 +1064,7 @@
       </c>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1063,7 +1091,7 @@
       </c>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1090,7 +1118,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -1117,7 +1145,7 @@
       </c>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -1144,7 +1172,7 @@
       </c>
       <c r="I11" s="12"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -1171,7 +1199,7 @@
       </c>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -1198,7 +1226,7 @@
       </c>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -1225,7 +1253,7 @@
       </c>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1252,7 +1280,7 @@
       </c>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -1279,7 +1307,7 @@
       </c>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1">
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -1306,7 +1334,7 @@
       </c>
       <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1">
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -1333,7 +1361,7 @@
       </c>
       <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1">
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -1360,7 +1388,7 @@
       </c>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1">
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -1387,7 +1415,7 @@
       </c>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1">
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -1414,7 +1442,7 @@
       </c>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1">
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -1439,109 +1467,113 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A23" s="14">
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12">
         <v>22</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="H23" s="16" t="s">
+      <c r="H23" s="9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A24" s="14">
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12">
         <v>23</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="G24" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="16" t="s">
+      <c r="H24" s="9" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A25" s="14">
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12">
         <v>24</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="G25" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A26" s="14">
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12">
         <v>25</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="G26" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="9" t="s">
         <v>126</v>
       </c>
+      <c r="I26" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>